<commit_message>
Aumento de limite en Descr Enfermedad y Descr Peste
</commit_message>
<xml_diff>
--- a/Diccionario de datos/diccDatos.xlsx
+++ b/Diccionario de datos/diccDatos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ale\Documents\Universidad\Segundo cuatri 2022\Lenguajes de bases de datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Documents\GitHub\ProyectoVivero\Diccionario de datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8B8A1FD-32D8-4CA8-90EA-163975A7CC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB01AB8-0C6C-40B8-BEE7-CFD28D0DCD23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5235" yWindow="3120" windowWidth="21600" windowHeight="11325" xr2:uid="{DAC34EB2-D53D-4CE5-BA09-C8DEC67FB6D9}"/>
+    <workbookView xWindow="2430" yWindow="2625" windowWidth="25890" windowHeight="17370" xr2:uid="{DAC34EB2-D53D-4CE5-BA09-C8DEC67FB6D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -656,7 +656,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,7 +825,7 @@
         <v>21</v>
       </c>
       <c r="B12">
-        <v>100</v>
+        <v>350</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -965,7 +965,7 @@
         <v>45</v>
       </c>
       <c r="B22">
-        <v>100</v>
+        <v>350</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Adicion Carpeta Imagenes + Actualizacion limite columna REGION
</commit_message>
<xml_diff>
--- a/Diccionario de datos/diccDatos.xlsx
+++ b/Diccionario de datos/diccDatos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Documents\GitHub\ProyectoVivero\Diccionario de datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB01AB8-0C6C-40B8-BEE7-CFD28D0DCD23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5251637D-5B70-4C50-A9B0-02E084AEA382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2430" yWindow="2625" windowWidth="25890" windowHeight="17370" xr2:uid="{DAC34EB2-D53D-4CE5-BA09-C8DEC67FB6D9}"/>
   </bookViews>
@@ -656,7 +656,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1203,7 +1203,7 @@
         <v>81</v>
       </c>
       <c r="B39">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C39" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Adicion de columna Toxicidad a diccionario
</commit_message>
<xml_diff>
--- a/Diccionario de datos/diccDatos.xlsx
+++ b/Diccionario de datos/diccDatos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexa\Documents\GitHub\ProyectoVivero\Diccionario de datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5251637D-5B70-4C50-A9B0-02E084AEA382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E30B78-82A1-45BC-8B58-4B8805A315D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2430" yWindow="2625" windowWidth="25890" windowHeight="17370" xr2:uid="{DAC34EB2-D53D-4CE5-BA09-C8DEC67FB6D9}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="91">
   <si>
     <t>Campo</t>
   </si>
@@ -302,6 +302,12 @@
   </si>
   <si>
     <t>Tipo general de la planta actual (arbol, hongo, cactus, flor)</t>
+  </si>
+  <si>
+    <t>toxicidad</t>
+  </si>
+  <si>
+    <t>Nivel de toxicidad de pla planta.</t>
   </si>
 </sst>
 </file>
@@ -653,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAA8D0CF-51BD-43DA-84B8-E575D5C266C1}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,6 +1260,20 @@
         <v>88</v>
       </c>
     </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>89</v>
+      </c>
+      <c r="B43">
+        <v>50</v>
+      </c>
+      <c r="C43" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43" t="s">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>